<commit_message>
BAJAJ & MAGMA FILES
</commit_message>
<xml_diff>
--- a/media/BAJAJ-PL/Billing/FEB 22/BAJAJ-PL Billing MIS.xlsx
+++ b/media/BAJAJ-PL/Billing/FEB 22/BAJAJ-PL Billing MIS.xlsx
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>61254.75</v>
+        <v>67398.14999999999</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>33710.56</v>
+        <v>38094.56</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>28380.82</v>
+        <v>31786.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>